<commit_message>
correction to previous commit
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Obsidian\Nico\4._Development_and_IT\01-Code_Snippets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\host\znpepin (192.168.15.1)\Projects\Collection-of-CSharp-ExcelDNA-UDFs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E51949A-1A20-477A-B504-1C90FFBC3CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB92E9C9-77CC-45DC-B39D-3D5A2A459989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14066" xr2:uid="{61C619A1-3838-47F4-8649-F8150DB55F41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="48"/>
+  <calcPr calcId="191029" concurrentManualCount="24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -211,17 +211,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9328A7-B952-46DD-A482-20174246AFE2}">
   <dimension ref="A4:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -568,20 +565,20 @@
     <col min="3" max="3" width="23.234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>16</v>
       </c>
@@ -596,28 +593,22 @@
         <v>btlCxRWOLKFSXMBX</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="str" cm="1">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="str" cm="1">
         <f t="array" ref="D6">_xll.HashArray(B6:C6, A6)</f>
         <v>8xY8N3VsmMGrudb6</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>32</v>
       </c>
@@ -632,68 +623,52 @@
         <v>btlCxRWOLKFSXMBXy2fhXc5iCyqKWIvR</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="str" cm="1">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">_xll.HashArray(B8:C8, A8)</f>
         <v>8xY8N3VsmMGrudb68jEc49FNXqMlTlBv</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8" t="b">
+      <c r="B9" s="6" t="b">
         <f>AND(D5=D6,D7=D8)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A11" s="6" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
@@ -704,77 +679,72 @@
         <v>Using cached thread settings</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="str" cm="1">
-        <f t="array" aca="1" ref="A15:B17" ca="1">_xll.GetThreads()</f>
+        <f t="array" ref="A15:B17">_xll.GetThreads()</f>
         <v>Current Thread Count</v>
       </c>
       <c r="B15">
-        <f ca="1"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="str">
-        <f ca="1"/>
         <v>Max Available</v>
       </c>
       <c r="B16">
-        <f ca="1"/>
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" t="str">
-        <f ca="1"/>
         <v>Mode Enabled</v>
       </c>
       <c r="B17" t="b">
-        <f ca="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="5" t="b">
-        <f ca="1">B15=B12</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="3" t="b">
+        <f>B15=B12</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
@@ -819,20 +789,20 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5" t="b">
+      <c r="B24" s="3" t="b">
         <f>AND(B21,B22,NOT(B23))</f>
         <v>1</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
@@ -888,7 +858,7 @@
       <c r="G28" t="str">
         <v>ddddd</v>
       </c>
-      <c r="H28" s="9" t="str">
+      <c r="H28" t="str">
         <v/>
       </c>
       <c r="I28" t="str">
@@ -902,20 +872,20 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="5" t="b">
+      <c r="B31" s="3" t="b">
         <f>AND(C27=C26,C29=C28)</f>
         <v>1</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
@@ -1012,20 +982,20 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="5" t="b">
+      <c r="B40" s="3" t="b">
         <f>AND(A34=D34,A35=D35,A36=D36,A37=D37,ISERR(D38))</f>
         <v>1</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>